<commit_message>
Finalisation of first model with fit plot
</commit_message>
<xml_diff>
--- a/inputs/data/Metadata_Table.xlsx
+++ b/inputs/data/Metadata_Table.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\MorphometricsALB\inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01DAB8E5-D49D-4DDB-82AA-360172703BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AC7556-5F37-4AD0-A02C-B6DC8A8648D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26895" yWindow="1005" windowWidth="21600" windowHeight="11385" xr2:uid="{9C546C02-3B0F-4898-8ACE-CED84A4C9EDE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9C546C02-3B0F-4898-8ACE-CED84A4C9EDE}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Field</t>
   </si>
@@ -161,6 +161,12 @@
   </si>
   <si>
     <t>[Well-known text of the geometry](http://wiki.gis.com/wiki/index.php/Well-known_text)</t>
+  </si>
+  <si>
+    <t>CAPTURE_QUARTER</t>
+  </si>
+  <si>
+    <t>Quarter of the "average" date of capture</t>
   </si>
 </sst>
 </file>
@@ -532,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A541981-7735-4597-88E9-80ADD3A3E605}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,49 +671,57 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>10</v>
+        <v>42</v>
       </c>
       <c r="B15" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" t="s">
-        <v>23</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>22</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>24</v>
       </c>
     </row>

</xml_diff>

<commit_message>
progress in M&M writing
</commit_message>
<xml_diff>
--- a/inputs/data/Metadata_Table.xlsx
+++ b/inputs/data/Metadata_Table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\echassot\Desktop\MorphometricsALB\inputs\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65AC7556-5F37-4AD0-A02C-B6DC8A8648D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{299F6A51-969A-4FDF-B50D-4BB04A435410}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9C546C02-3B0F-4898-8ACE-CED84A4C9EDE}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>Field</t>
   </si>
@@ -46,9 +46,6 @@
     <t>SOURCE</t>
   </si>
   <si>
-    <t>Institution of origin of the data (e.g., MUS University-IRD)</t>
-  </si>
-  <si>
     <t>PROJECT</t>
   </si>
   <si>
@@ -70,12 +67,6 @@
     <t>SAMPLING_PLATFORM</t>
   </si>
   <si>
-    <t>Maximum date of capture of the fish</t>
-  </si>
-  <si>
-    <t>Minimum date of capture of the fish</t>
-  </si>
-  <si>
     <t>FISHERY_CODE</t>
   </si>
   <si>
@@ -142,9 +133,6 @@
     <t>IOTC label for the fishery</t>
   </si>
   <si>
-    <t>CWP grid code or area name (Chagos archipelago) when not available</t>
-  </si>
-  <si>
     <t>http://wiki.gis.com/wiki/index.php/Well-known_text</t>
   </si>
   <si>
@@ -160,13 +148,49 @@
     <t>Sex of the fish derived from macroscopic exam. M = Male; F = Female; I = Indeterminate; U = Unknown</t>
   </si>
   <si>
-    <t>[Well-known text of the geometry](http://wiki.gis.com/wiki/index.php/Well-known_text)</t>
-  </si>
-  <si>
     <t>CAPTURE_QUARTER</t>
   </si>
   <si>
-    <t>Quarter of the "average" date of capture</t>
+    <t>CWP grid code or area name when not available</t>
+  </si>
+  <si>
+    <t>Institution of origin of the data</t>
+  </si>
+  <si>
+    <t>LON_CENTROID</t>
+  </si>
+  <si>
+    <t>LAT_CENTROID</t>
+  </si>
+  <si>
+    <t>Latitude (decimal degrees) of the centroid of the fishing ground</t>
+  </si>
+  <si>
+    <t>Longitude (decimal degrees) of the centroid of the fishing ground</t>
+  </si>
+  <si>
+    <t>Minimum date of capture of the fish (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>Maximum date of capture of the fish (YYYY-MM-DD)</t>
+  </si>
+  <si>
+    <t>Quarter of the "average" date of capture: 1, 2, 3, 4</t>
+  </si>
+  <si>
+    <t>log10FL</t>
+  </si>
+  <si>
+    <t>log10RD</t>
+  </si>
+  <si>
+    <t>Logarithm to base 10 of fork length</t>
+  </si>
+  <si>
+    <t>Logarithm to base 10 of round weight</t>
+  </si>
+  <si>
+    <t>Well-known text of the geometry</t>
   </si>
 </sst>
 </file>
@@ -538,10 +562,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1A541981-7735-4597-88E9-80ADD3A3E605}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -561,10 +585,10 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
-      </c>
-      <c r="B2" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -572,157 +596,191 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>8</v>
+        <v>40</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
-      </c>
+        <v>43</v>
+      </c>
+      <c r="C13" s="2"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>9</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
-      </c>
+        <v>42</v>
+      </c>
+      <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>